<commit_message>
Match T1w not T1
</commit_message>
<xml_diff>
--- a/config/afirm_config.xlsx
+++ b/config/afirm_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\martin\code\xnat-imgqc\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C2A8D2B-9BC7-45F9-94FE-61498FE19291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2C3A7A-7EF1-4D3E-BF29-52574ECEF0CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="2625" windowWidth="25545" windowHeight="13395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="435" windowWidth="20490" windowHeight="10335" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checks" sheetId="1" r:id="rId1"/>
@@ -35,17 +35,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
-  <si>
-    <t>2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Test</t>
   </si>
   <si>
-    <t>T1</t>
-  </si>
-  <si>
     <t>isnr</t>
   </si>
   <si>
@@ -71,6 +65,9 @@
   </si>
   <si>
     <t>T2w</t>
+  </si>
+  <si>
+    <t>T1w</t>
   </si>
 </sst>
 </file>
@@ -122,7 +119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -140,10 +137,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -430,7 +424,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,69 +441,51 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>2</v>
       </c>
       <c r="B2" s="6"/>
       <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="4">
-        <v>3</v>
-      </c>
-      <c r="H2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="7"/>
+        <v>9</v>
+      </c>
+      <c r="B3" s="6"/>
       <c r="D3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3">
         <v>1</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="4">
-        <v>3</v>
-      </c>
-      <c r="H3">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
+      <c r="B4" s="6"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
@@ -525,7 +501,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
+      <c r="B8" s="6"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D9"/>
@@ -714,12 +690,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -728,7 +698,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F57573F99DE79145B2C4B20841E12603" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bffb4cedf0b3900262138fdae33e2dc4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0c1e910d-4918-42f1-af2c-ed1101d63abc" xmlns:ns4="786e620f-b1da-4f59-878c-ef7546d25bf1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="37173867f386110bdd2a41aaff59b7e1" ns3:_="" ns4:_="">
     <xsd:import namespace="0c1e910d-4918-42f1-af2c-ed1101d63abc"/>
@@ -957,24 +927,13 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D40F5F12-58EE-4BA1-8910-4436D8D8475A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="786e620f-b1da-4f59-878c-ef7546d25bf1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="0c1e910d-4918-42f1-af2c-ed1101d63abc"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FE73DB8-1736-4671-8FD3-622DFFD73211}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -982,7 +941,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4D01498-1E58-48D4-ACAD-5E74F94105E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -999,4 +958,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D40F5F12-58EE-4BA1-8910-4436D8D8475A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="786e620f-b1da-4f59-878c-ef7546d25bf1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0c1e910d-4918-42f1-af2c-ed1101d63abc"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>